<commit_message>
Moved simulation into System Model folder
Originally in Software folder, but that was not correct
</commit_message>
<xml_diff>
--- a/System Modelling/Mechanical/Finite Elements/Force Calculations.xlsx
+++ b/System Modelling/Mechanical/Finite Elements/Force Calculations.xlsx
@@ -756,16 +756,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="0" style="3" hidden="1" customWidth="1"/>
-    <col min="6" max="11" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="2" width="8.88671875" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="3" customWidth="1"/>
+    <col min="6" max="11" width="8.88671875" customWidth="1"/>
     <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Updated dynamics summary and matlab files
Dynamics summary is 10 pages and still needs references/sources
Updated matlab files to calculate impulse foot forces
Added a summary table to force calculations for report
</commit_message>
<xml_diff>
--- a/System Modelling/Mechanical/Finite Elements/Force Calculations.xlsx
+++ b/System Modelling/Mechanical/Finite Elements/Force Calculations.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="64">
   <si>
     <t>TI1 =</t>
   </si>
@@ -208,6 +208,15 @@
   </si>
   <si>
     <t>value</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>Drag</t>
+  </si>
+  <si>
+    <t>Impulse</t>
   </si>
 </sst>
 </file>
@@ -410,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -480,6 +489,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -760,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O96"/>
+  <dimension ref="A1:Q96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10:L11"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -775,7 +787,7 @@
     <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -800,8 +812,20 @@
       <c r="L1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>7</v>
       </c>
@@ -825,8 +849,20 @@
       <c r="I2">
         <v>-76.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" s="45">
+        <v>383.20080000000002</v>
+      </c>
+      <c r="P2" s="45">
+        <v>67.081999999999994</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -838,8 +874,20 @@
         <v>2.9007999999999998</v>
       </c>
       <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="O3" s="45">
+        <v>2.9007999999999998</v>
+      </c>
+      <c r="P3" s="45">
+        <v>-3.1366999999999998</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -851,8 +899,20 @@
         <v>-0.7823</v>
       </c>
       <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="O4" s="45">
+        <v>-0.7823</v>
+      </c>
+      <c r="P4" s="45">
+        <v>-1.3573</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -869,8 +929,20 @@
       <c r="F5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="O5" s="45">
+        <v>2.9007999999999998</v>
+      </c>
+      <c r="P5" s="45">
+        <v>-3.1366999999999998</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
@@ -888,8 +960,20 @@
         <f>B6/E6</f>
         <v>7.7264705882352933</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O6" s="45">
+        <v>1.3134999999999999</v>
+      </c>
+      <c r="P6" s="45">
+        <v>99.325299999999999</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -900,8 +984,20 @@
         <f t="shared" si="0"/>
         <v>17.5289</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O7" s="45">
+        <v>17.5289</v>
+      </c>
+      <c r="P7" s="45">
+        <v>6.8914</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -912,8 +1008,20 @@
         <f t="shared" si="0"/>
         <v>-13.2918</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O8" s="45">
+        <v>-13.2918</v>
+      </c>
+      <c r="P8" s="45">
+        <v>-9.8417999999999992</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -930,8 +1038,20 @@
       <c r="I9" s="8">
         <v>138</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O9" s="45">
+        <v>17.5289</v>
+      </c>
+      <c r="P9" s="45">
+        <v>6.8914</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="H10" s="10" t="s">
         <v>40</v>
@@ -945,8 +1065,22 @@
       <c r="L10" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O10" s="3">
+        <f>C50</f>
+        <v>557.6</v>
+      </c>
+      <c r="P10" s="3">
+        <f>Drag!D27</f>
+        <v>33.709200000000003</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>12.386900000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="K11">
         <v>-70.099999999999994</v>
@@ -954,11 +1088,39 @@
       <c r="L11">
         <v>-85.1</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O11" s="3">
+        <f t="shared" ref="O11:O25" si="1">C51</f>
+        <v>911</v>
+      </c>
+      <c r="P11" s="3">
+        <f>Drag!D28</f>
+        <v>91.940799999999996</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O12" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P12" s="3">
+        <f>Drag!D29</f>
+        <v>17.25</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>59</v>
       </c>
@@ -978,8 +1140,22 @@
         <f>0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O13" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P13" s="3">
+        <f>Drag!D30</f>
+        <v>17.25</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>7</v>
       </c>
@@ -1003,8 +1179,22 @@
       <c r="I14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O14" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P14" s="3">
+        <f>Drag!D31</f>
+        <v>17.25</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1012,7 +1202,7 @@
         <v>2.9007999999999998</v>
       </c>
       <c r="C15">
-        <f t="shared" ref="C15:C21" si="1">B15</f>
+        <f t="shared" ref="C15:C21" si="2">B15</f>
         <v>2.9007999999999998</v>
       </c>
       <c r="E15" s="2"/>
@@ -1022,8 +1212,22 @@
       <c r="I15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O15" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P15" s="3">
+        <f>Drag!D32</f>
+        <v>17.25</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1031,7 +1235,7 @@
         <v>-0.7823</v>
       </c>
       <c r="C16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.7823</v>
       </c>
       <c r="E16" s="2"/>
@@ -1041,8 +1245,22 @@
       <c r="I16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P16" s="3">
+        <f>Drag!D33</f>
+        <v>17.25</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1050,7 +1268,7 @@
         <v>2.9007999999999998</v>
       </c>
       <c r="C17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.9007999999999998</v>
       </c>
       <c r="E17" s="2" t="s">
@@ -1066,8 +1284,22 @@
         <f>0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O17" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P17" s="3">
+        <f>Drag!D34</f>
+        <v>17.25</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>5</v>
       </c>
@@ -1075,7 +1307,7 @@
         <v>55.8459</v>
       </c>
       <c r="C18" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>55.8459</v>
       </c>
       <c r="E18" s="2">
@@ -1092,8 +1324,23 @@
         <f>I9/3</f>
         <v>46</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O18" s="3">
+        <f t="shared" si="1"/>
+        <v>789.90000000000009</v>
+      </c>
+      <c r="P18" s="3">
+        <f>Drag!D35</f>
+        <v>145.80549999999999</v>
+      </c>
+      <c r="Q18" s="3">
+        <f>15.8962+I9/4</f>
+        <v>50.3962</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1101,7 +1348,7 @@
         <v>17.5289</v>
       </c>
       <c r="C19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17.5289</v>
       </c>
       <c r="H19" t="s">
@@ -1111,8 +1358,23 @@
         <f>I9/3</f>
         <v>46</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O19" s="3">
+        <f t="shared" si="1"/>
+        <v>1321.1999999999998</v>
+      </c>
+      <c r="P19" s="3">
+        <f>Drag!D36</f>
+        <v>199.8142</v>
+      </c>
+      <c r="Q19" s="3">
+        <f t="shared" ref="Q19:Q25" si="3">$I$9/4</f>
+        <v>34.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -1120,7 +1382,7 @@
         <v>-13.2918</v>
       </c>
       <c r="C20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-13.2918</v>
       </c>
       <c r="H20" t="s">
@@ -1130,8 +1392,23 @@
         <f>I9/3</f>
         <v>46</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O20" s="3">
+        <f t="shared" si="1"/>
+        <v>-42.4</v>
+      </c>
+      <c r="P20" s="3">
+        <f>Drag!D37</f>
+        <v>30.8703</v>
+      </c>
+      <c r="Q20" s="3">
+        <f t="shared" si="3"/>
+        <v>34.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1139,20 +1416,80 @@
         <v>17.5289</v>
       </c>
       <c r="C21">
+        <f t="shared" si="2"/>
+        <v>17.5289</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O21" s="3">
         <f t="shared" si="1"/>
-        <v>17.5289</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+        <v>-38.199999999999996</v>
+      </c>
+      <c r="P21" s="3">
+        <f>Drag!D38</f>
+        <v>26.652000000000001</v>
+      </c>
+      <c r="Q21" s="3">
+        <f t="shared" si="3"/>
+        <v>34.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O22" s="3">
+        <f t="shared" si="1"/>
+        <v>-42.4</v>
+      </c>
+      <c r="P22" s="3">
+        <f>Drag!D39</f>
+        <v>30.8703</v>
+      </c>
+      <c r="Q22" s="3">
+        <f t="shared" si="3"/>
+        <v>34.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O23" s="3">
+        <f t="shared" si="1"/>
+        <v>-38.199999999999996</v>
+      </c>
+      <c r="P23" s="3">
+        <f>Drag!D40</f>
+        <v>26.652000000000001</v>
+      </c>
+      <c r="Q23" s="3">
+        <f t="shared" si="3"/>
+        <v>34.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N24" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O24" s="3">
+        <f t="shared" si="1"/>
+        <v>-42.4</v>
+      </c>
+      <c r="P24" s="3">
+        <f>Drag!D41</f>
+        <v>30.8703</v>
+      </c>
+      <c r="Q24" s="3">
+        <f t="shared" si="3"/>
+        <v>34.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>49</v>
       </c>
@@ -1163,8 +1500,23 @@
       <c r="I25" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N25" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O25" s="3">
+        <f t="shared" si="1"/>
+        <v>-38.199999999999996</v>
+      </c>
+      <c r="P25" s="3">
+        <f>Drag!D42</f>
+        <v>26.652000000000001</v>
+      </c>
+      <c r="Q25" s="3">
+        <f t="shared" si="3"/>
+        <v>34.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B26" s="13" t="s">
         <v>3</v>
       </c>
@@ -1174,14 +1526,15 @@
       <c r="I26">
         <v>-76.5</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N26" s="3"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B27" s="6"/>
       <c r="L27" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>13</v>
       </c>
@@ -1205,7 +1558,7 @@
         <v>-140.86528368380002</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
         <v>14</v>
       </c>
@@ -1213,20 +1566,20 @@
         <v>-0.78300000000000003</v>
       </c>
       <c r="C29" s="12">
-        <f t="shared" ref="C29:C43" si="2">B29*1000</f>
+        <f t="shared" ref="C29:C43" si="4">B29*1000</f>
         <v>-783</v>
       </c>
       <c r="D29" s="12">
-        <f t="shared" ref="D29:D43" si="3">ABS(C29)</f>
+        <f t="shared" ref="D29:D43" si="5">ABS(C29)</f>
         <v>783</v>
       </c>
       <c r="E29" s="44"/>
       <c r="L29">
-        <f t="shared" ref="L29:L43" si="4">C29*0.224808943</f>
+        <f t="shared" ref="L29:L43" si="6">C29*0.224808943</f>
         <v>-176.02540236900001</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>15</v>
       </c>
@@ -1234,20 +1587,20 @@
         <v>0</v>
       </c>
       <c r="C30" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="D30" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E30" s="7"/>
       <c r="L30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -1255,20 +1608,20 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="D31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E31" s="2"/>
       <c r="L31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>17</v>
       </c>
@@ -1276,16 +1629,16 @@
         <v>0</v>
       </c>
       <c r="C32" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="D32" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E32" s="7"/>
       <c r="L32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -1297,16 +1650,16 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="D33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E33" s="2"/>
       <c r="L33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -1318,16 +1671,16 @@
         <v>0</v>
       </c>
       <c r="C34" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="D34" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E34" s="7"/>
       <c r="L34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -1339,16 +1692,16 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="D35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E35" s="2"/>
       <c r="L35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -1360,16 +1713,16 @@
         <v>0.80679999999999996</v>
       </c>
       <c r="C36" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>806.8</v>
       </c>
       <c r="D36" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>806.8</v>
       </c>
       <c r="E36" s="7"/>
       <c r="L36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>181.37585521240001</v>
       </c>
     </row>
@@ -1381,16 +1734,16 @@
         <v>1.1418999999999999</v>
       </c>
       <c r="C37" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1141.8999999999999</v>
       </c>
       <c r="D37" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1141.8999999999999</v>
       </c>
       <c r="E37" s="44"/>
       <c r="L37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>256.70933201169998</v>
       </c>
     </row>
@@ -1402,16 +1755,16 @@
         <v>-4.24E-2</v>
       </c>
       <c r="C38" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-42.4</v>
       </c>
       <c r="D38" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>42.4</v>
       </c>
       <c r="E38" s="7"/>
       <c r="L38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-9.5318991832000002</v>
       </c>
     </row>
@@ -1423,16 +1776,16 @@
         <v>-3.8199999999999998E-2</v>
       </c>
       <c r="C39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-38.199999999999996</v>
       </c>
       <c r="D39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>38.199999999999996</v>
       </c>
       <c r="E39" s="2"/>
       <c r="L39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-8.5877016225999991</v>
       </c>
     </row>
@@ -1444,16 +1797,16 @@
         <v>-4.24E-2</v>
       </c>
       <c r="C40" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-42.4</v>
       </c>
       <c r="D40" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>42.4</v>
       </c>
       <c r="E40" s="7"/>
       <c r="L40">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-9.5318991832000002</v>
       </c>
     </row>
@@ -1465,16 +1818,16 @@
         <v>-3.8199999999999998E-2</v>
       </c>
       <c r="C41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-38.199999999999996</v>
       </c>
       <c r="D41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>38.199999999999996</v>
       </c>
       <c r="E41" s="2"/>
       <c r="L41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-8.5877016225999991</v>
       </c>
     </row>
@@ -1486,16 +1839,16 @@
         <v>-4.24E-2</v>
       </c>
       <c r="C42" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-42.4</v>
       </c>
       <c r="D42" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>42.4</v>
       </c>
       <c r="E42" s="7"/>
       <c r="L42">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-9.5318991832000002</v>
       </c>
     </row>
@@ -1507,16 +1860,16 @@
         <v>-3.8199999999999998E-2</v>
       </c>
       <c r="C43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-38.199999999999996</v>
       </c>
       <c r="D43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>38.199999999999996</v>
       </c>
       <c r="E43" s="2"/>
       <c r="L43">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-8.5877016225999991</v>
       </c>
     </row>
@@ -1581,7 +1934,7 @@
         <v>-85.1</v>
       </c>
       <c r="L50">
-        <f t="shared" ref="L50:L65" si="5">C50*0.224808943</f>
+        <f t="shared" ref="L50:L65" si="7">C50*0.224808943</f>
         <v>125.35346661680001</v>
       </c>
       <c r="M50" t="s">
@@ -1596,16 +1949,16 @@
         <v>0.91100000000000003</v>
       </c>
       <c r="C51">
-        <f t="shared" ref="C51:C65" si="6">1000*B51</f>
+        <f t="shared" ref="C51:C65" si="8">1000*B51</f>
         <v>911</v>
       </c>
       <c r="D51">
-        <f t="shared" ref="D51:D65" si="7">ABS(C51)</f>
+        <f t="shared" ref="D51:D65" si="9">ABS(C51)</f>
         <v>911</v>
       </c>
       <c r="E51" s="2"/>
       <c r="L51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>204.800947073</v>
       </c>
       <c r="M51" t="s">
@@ -1623,16 +1976,16 @@
         <v>0</v>
       </c>
       <c r="C52" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D52" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="E52" s="2"/>
       <c r="L52">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="O52" t="s">
@@ -1647,16 +2000,16 @@
         <v>0</v>
       </c>
       <c r="C53">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D53">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="E53" s="2"/>
       <c r="L53">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -1668,16 +2021,16 @@
         <v>0</v>
       </c>
       <c r="C54" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D54" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="E54" s="2"/>
       <c r="L54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -1689,16 +2042,16 @@
         <v>0</v>
       </c>
       <c r="C55">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D55">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="E55" s="2"/>
       <c r="L55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -1710,16 +2063,16 @@
         <v>0</v>
       </c>
       <c r="C56" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D56" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="E56" s="2"/>
       <c r="L56">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -1731,16 +2084,16 @@
         <v>0</v>
       </c>
       <c r="C57">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D57">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="E57" s="2"/>
       <c r="L57">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -1752,16 +2105,16 @@
         <v>0.78990000000000005</v>
       </c>
       <c r="C58" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>789.90000000000009</v>
       </c>
       <c r="D58" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>789.90000000000009</v>
       </c>
       <c r="E58" s="2"/>
       <c r="L58">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>177.57658407570003</v>
       </c>
       <c r="M58" t="s">
@@ -1776,16 +2129,16 @@
         <v>1.3211999999999999</v>
       </c>
       <c r="C59">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1321.1999999999998</v>
       </c>
       <c r="D59">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1321.1999999999998</v>
       </c>
       <c r="E59" s="2"/>
       <c r="L59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>297.01757549159998</v>
       </c>
       <c r="M59" t="s">
@@ -1800,16 +2153,16 @@
         <v>-4.24E-2</v>
       </c>
       <c r="C60" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-42.4</v>
       </c>
       <c r="D60" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>42.4</v>
       </c>
       <c r="E60" s="2"/>
       <c r="L60">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-9.5318991832000002</v>
       </c>
     </row>
@@ -1821,16 +2174,16 @@
         <v>-3.8199999999999998E-2</v>
       </c>
       <c r="C61">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-38.199999999999996</v>
       </c>
       <c r="D61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>38.199999999999996</v>
       </c>
       <c r="E61" s="2"/>
       <c r="L61">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-8.5877016225999991</v>
       </c>
     </row>
@@ -1842,16 +2195,16 @@
         <v>-4.24E-2</v>
       </c>
       <c r="C62" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-42.4</v>
       </c>
       <c r="D62" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>42.4</v>
       </c>
       <c r="E62" s="2"/>
       <c r="L62">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-9.5318991832000002</v>
       </c>
     </row>
@@ -1863,16 +2216,16 @@
         <v>-3.8199999999999998E-2</v>
       </c>
       <c r="C63">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-38.199999999999996</v>
       </c>
       <c r="D63">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>38.199999999999996</v>
       </c>
       <c r="E63" s="2"/>
       <c r="L63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-8.5877016225999991</v>
       </c>
     </row>
@@ -1884,16 +2237,16 @@
         <v>-4.24E-2</v>
       </c>
       <c r="C64" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-42.4</v>
       </c>
       <c r="D64" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>42.4</v>
       </c>
       <c r="E64" s="2"/>
       <c r="L64">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-9.5318991832000002</v>
       </c>
     </row>
@@ -1905,16 +2258,16 @@
         <v>-3.8199999999999998E-2</v>
       </c>
       <c r="C65">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-38.199999999999996</v>
       </c>
       <c r="D65">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>38.199999999999996</v>
       </c>
       <c r="E65" s="2"/>
       <c r="L65">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-8.5877016225999991</v>
       </c>
     </row>
@@ -2021,8 +2374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J94"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>